<commit_message>
Finshing the structure of MatchCatCode and starting te plotting code
</commit_message>
<xml_diff>
--- a/CBi_NOR_test.xlsx
+++ b/CBi_NOR_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\GVX0EPF00012AAF\EXCELCNV\449c4a51-56db-49f3-9261-a52056c49e13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{796F0D2E-9A17-44FC-92FF-D4FD08C9E254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59613EA1-C5A3-4441-AF5D-823B77E0EC6B}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{796F0D2E-9A17-44FC-92FF-D4FD08C9E254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B115F45-6567-4809-AA02-617574C0123F}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{3D9E6229-9C3C-458A-B3D7-07608300DC4A}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <t>Printed matter and recorded media (22)</t>
   </si>
   <si>
-    <t>Coke and Tar</t>
+    <t>Coke and tar</t>
   </si>
   <si>
     <t>Petroleum products</t>
@@ -1160,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E997B41-1F61-4333-82E5-27F5D3409912}">
   <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Nothing special, just collecting some data
</commit_message>
<xml_diff>
--- a/CBi_NOR_test.xlsx
+++ b/CBi_NOR_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\GVX0EPF00012AAF\EXCELCNV\449c4a51-56db-49f3-9261-a52056c49e13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{796F0D2E-9A17-44FC-92FF-D4FD08C9E254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B115F45-6567-4809-AA02-617574C0123F}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{796F0D2E-9A17-44FC-92FF-D4FD08C9E254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99CC5C29-57E2-49BF-82FD-5AF60853D416}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{3D9E6229-9C3C-458A-B3D7-07608300DC4A}"/>
   </bookViews>
@@ -95,7 +95,7 @@
     <t>Meat products</t>
   </si>
   <si>
-    <t>Products of vegetable oils and fats</t>
+    <t>products of Vegetable oils and fats</t>
   </si>
   <si>
     <t>Dairy products</t>
@@ -119,7 +119,7 @@
     <t>Printed matter and recorded media (22)</t>
   </si>
   <si>
-    <t>Coke and tar</t>
+    <t>Coke and Tar</t>
   </si>
   <si>
     <t>Petroleum products</t>
@@ -1160,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E997B41-1F61-4333-82E5-27F5D3409912}">
   <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>

</xml_diff>